<commit_message>
Add dates to excell
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Eile</t>
   </si>
@@ -25,7 +25,22 @@
     <t>Kiekis</t>
   </si>
   <si>
+    <t>DATE</t>
+  </si>
+  <si>
     <t>Viso</t>
+  </si>
+  <si>
+    <t>2021/10/24</t>
+  </si>
+  <si>
+    <t>2024 - 12 - 10</t>
+  </si>
+  <si>
+    <t>2021\10\24</t>
+  </si>
+  <si>
+    <t>2021 - 10 - 24</t>
   </si>
   <si>
     <t>Iš viso</t>
@@ -360,13 +375,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -379,8 +394,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -390,12 +408,15 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2">
         <f>B2*C2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -405,12 +426,15 @@
       <c r="C3">
         <v>5</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3">
         <f>B3*C3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -420,12 +444,15 @@
       <c r="C4">
         <v>4</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4">
         <f>B4*C4</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -435,12 +462,15 @@
       <c r="C5">
         <v>4</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5">
         <f>B5*C5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -450,14 +480,17 @@
       <c r="C6">
         <v>3</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6">
         <f>B6*C6</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <f>SUM(B2:B6)</f>
@@ -467,8 +500,11 @@
         <f>SUM(C2:C6)</f>
         <v>0</v>
       </c>
-      <c r="D7">
-        <f>SUM(D2:D6)</f>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <f>SUM(E2:E6)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>